<commit_message>
Fix tests and other trello changes
</commit_message>
<xml_diff>
--- a/test-data/input/test-data-input-xls-mult-feb.xlsx
+++ b/test-data/input/test-data-input-xls-mult-feb.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
-  <workbookPr defaultThemeVersion="124226"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <workbookPr/>
+  <workbookProtection/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
+  <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="4">
   <si>
     <t>cost</t>
   </si>
@@ -34,28 +35,23 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="YYYY-MM-DD HH:MM:SS"/>
+    <numFmt formatCode="yyyy-mm-dd h:mm:ss" numFmtId="164"/>
   </numFmts>
   <fonts count="2">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
+      <b val="1"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -70,36 +66,27 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="3">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf applyAlignment="1" borderId="1" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="164" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="0" hidden="0" name="Normal" xfId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
 </styleSheet>
 </file>
 
@@ -387,12 +374,18 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
@@ -409,157 +402,163 @@
       </c>
     </row>
     <row r="2" spans="1:4">
-      <c r="A2">
-        <v>-90</v>
-      </c>
-      <c r="B2" s="2">
+      <c r="A2" t="n">
+        <v>-90</v>
+      </c>
+      <c r="B2" s="2" t="n">
         <v>40575</v>
       </c>
-      <c r="C2">
-        <v>110</v>
-      </c>
-      <c r="D2">
+      <c r="C2" t="n">
+        <v>110</v>
+      </c>
+      <c r="D2" t="n">
         <v>200</v>
       </c>
     </row>
     <row r="3" spans="1:4">
-      <c r="A3">
-        <v>-90</v>
-      </c>
-      <c r="B3" s="2">
+      <c r="A3" t="n">
+        <v>-90</v>
+      </c>
+      <c r="B3" s="2" t="n">
         <v>40576</v>
       </c>
-      <c r="C3">
-        <v>110</v>
-      </c>
-      <c r="D3">
+      <c r="C3" t="n">
+        <v>110</v>
+      </c>
+      <c r="D3" t="n">
         <v>200</v>
       </c>
     </row>
     <row r="4" spans="1:4">
-      <c r="A4">
-        <v>-90</v>
-      </c>
-      <c r="B4" s="2">
+      <c r="A4" t="n">
+        <v>-90</v>
+      </c>
+      <c r="B4" s="2" t="n">
         <v>40577</v>
       </c>
-      <c r="C4">
-        <v>110</v>
-      </c>
-      <c r="D4">
+      <c r="C4" t="n">
+        <v>110</v>
+      </c>
+      <c r="D4" t="n">
         <v>200</v>
       </c>
     </row>
     <row r="5" spans="1:4">
-      <c r="A5">
-        <v>-90</v>
-      </c>
-      <c r="B5" s="2">
+      <c r="A5" t="n">
+        <v>-90</v>
+      </c>
+      <c r="B5" s="2" t="n">
         <v>40578</v>
       </c>
-      <c r="C5">
-        <v>110</v>
-      </c>
-      <c r="D5">
+      <c r="C5" t="n">
+        <v>110</v>
+      </c>
+      <c r="D5" t="n">
         <v>200</v>
       </c>
     </row>
     <row r="6" spans="1:4">
-      <c r="A6">
-        <v>-90</v>
-      </c>
-      <c r="B6" s="2">
+      <c r="A6" t="n">
+        <v>-90</v>
+      </c>
+      <c r="B6" s="2" t="n">
         <v>40579</v>
       </c>
-      <c r="C6">
-        <v>110</v>
-      </c>
-      <c r="D6">
+      <c r="C6" t="n">
+        <v>110</v>
+      </c>
+      <c r="D6" t="n">
         <v>200</v>
       </c>
     </row>
     <row r="7" spans="1:4">
-      <c r="A7">
-        <v>-90</v>
-      </c>
-      <c r="B7" s="2">
+      <c r="A7" t="n">
+        <v>-90</v>
+      </c>
+      <c r="B7" s="2" t="n">
         <v>40580</v>
       </c>
-      <c r="C7">
-        <v>110</v>
-      </c>
-      <c r="D7">
+      <c r="C7" t="n">
+        <v>110</v>
+      </c>
+      <c r="D7" t="n">
         <v>200</v>
       </c>
     </row>
     <row r="8" spans="1:4">
-      <c r="A8">
-        <v>-90</v>
-      </c>
-      <c r="B8" s="2">
+      <c r="A8" t="n">
+        <v>-90</v>
+      </c>
+      <c r="B8" s="2" t="n">
         <v>40581</v>
       </c>
-      <c r="C8">
-        <v>110</v>
-      </c>
-      <c r="D8">
+      <c r="C8" t="n">
+        <v>110</v>
+      </c>
+      <c r="D8" t="n">
         <v>200</v>
       </c>
     </row>
     <row r="9" spans="1:4">
-      <c r="A9">
-        <v>-90</v>
-      </c>
-      <c r="B9" s="2">
+      <c r="A9" t="n">
+        <v>-90</v>
+      </c>
+      <c r="B9" s="2" t="n">
         <v>40582</v>
       </c>
-      <c r="C9">
-        <v>110</v>
-      </c>
-      <c r="D9">
+      <c r="C9" t="n">
+        <v>110</v>
+      </c>
+      <c r="D9" t="n">
         <v>200</v>
       </c>
     </row>
     <row r="10" spans="1:4">
-      <c r="A10">
-        <v>-90</v>
-      </c>
-      <c r="B10" s="2">
+      <c r="A10" t="n">
+        <v>-90</v>
+      </c>
+      <c r="B10" s="2" t="n">
         <v>40583</v>
       </c>
-      <c r="C10">
-        <v>110</v>
-      </c>
-      <c r="D10">
+      <c r="C10" t="n">
+        <v>110</v>
+      </c>
+      <c r="D10" t="n">
         <v>200</v>
       </c>
     </row>
     <row r="11" spans="1:4">
-      <c r="A11">
-        <v>-90</v>
-      </c>
-      <c r="B11" s="2">
+      <c r="A11" t="n">
+        <v>-90</v>
+      </c>
+      <c r="B11" s="2" t="n">
         <v>40584</v>
       </c>
-      <c r="C11">
-        <v>110</v>
-      </c>
-      <c r="D11">
+      <c r="C11" t="n">
+        <v>110</v>
+      </c>
+      <c r="D11" t="n">
         <v>200</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
@@ -576,146 +575,146 @@
       </c>
     </row>
     <row r="2" spans="1:4">
-      <c r="A2">
-        <v>-90</v>
-      </c>
-      <c r="B2" s="2">
+      <c r="A2" t="n">
+        <v>-90</v>
+      </c>
+      <c r="B2" s="2" t="n">
         <v>40575</v>
       </c>
-      <c r="C2">
-        <v>110</v>
-      </c>
-      <c r="D2">
+      <c r="C2" t="n">
+        <v>110</v>
+      </c>
+      <c r="D2" t="n">
         <v>200</v>
       </c>
     </row>
     <row r="3" spans="1:4">
-      <c r="A3">
-        <v>-90</v>
-      </c>
-      <c r="B3" s="2">
+      <c r="A3" t="n">
+        <v>-90</v>
+      </c>
+      <c r="B3" s="2" t="n">
         <v>40576</v>
       </c>
-      <c r="C3">
-        <v>110</v>
-      </c>
-      <c r="D3">
+      <c r="C3" t="n">
+        <v>110</v>
+      </c>
+      <c r="D3" t="n">
         <v>200</v>
       </c>
     </row>
     <row r="4" spans="1:4">
-      <c r="A4">
-        <v>-90</v>
-      </c>
-      <c r="B4" s="2">
+      <c r="A4" t="n">
+        <v>-90</v>
+      </c>
+      <c r="B4" s="2" t="n">
         <v>40577</v>
       </c>
-      <c r="C4">
-        <v>110</v>
-      </c>
-      <c r="D4">
+      <c r="C4" t="n">
+        <v>110</v>
+      </c>
+      <c r="D4" t="n">
         <v>200</v>
       </c>
     </row>
     <row r="5" spans="1:4">
-      <c r="A5">
-        <v>-90</v>
-      </c>
-      <c r="B5" s="2">
+      <c r="A5" t="n">
+        <v>-90</v>
+      </c>
+      <c r="B5" s="2" t="n">
         <v>40578</v>
       </c>
-      <c r="C5">
-        <v>110</v>
-      </c>
-      <c r="D5">
+      <c r="C5" t="n">
+        <v>110</v>
+      </c>
+      <c r="D5" t="n">
         <v>200</v>
       </c>
     </row>
     <row r="6" spans="1:4">
-      <c r="A6">
-        <v>-90</v>
-      </c>
-      <c r="B6" s="2">
+      <c r="A6" t="n">
+        <v>-90</v>
+      </c>
+      <c r="B6" s="2" t="n">
         <v>40579</v>
       </c>
-      <c r="C6">
-        <v>110</v>
-      </c>
-      <c r="D6">
+      <c r="C6" t="n">
+        <v>110</v>
+      </c>
+      <c r="D6" t="n">
         <v>200</v>
       </c>
     </row>
     <row r="7" spans="1:4">
-      <c r="A7">
-        <v>-90</v>
-      </c>
-      <c r="B7" s="2">
+      <c r="A7" t="n">
+        <v>-90</v>
+      </c>
+      <c r="B7" s="2" t="n">
         <v>40580</v>
       </c>
-      <c r="C7">
-        <v>110</v>
-      </c>
-      <c r="D7">
+      <c r="C7" t="n">
+        <v>110</v>
+      </c>
+      <c r="D7" t="n">
         <v>200</v>
       </c>
     </row>
     <row r="8" spans="1:4">
-      <c r="A8">
-        <v>-90</v>
-      </c>
-      <c r="B8" s="2">
+      <c r="A8" t="n">
+        <v>-90</v>
+      </c>
+      <c r="B8" s="2" t="n">
         <v>40581</v>
       </c>
-      <c r="C8">
-        <v>110</v>
-      </c>
-      <c r="D8">
+      <c r="C8" t="n">
+        <v>110</v>
+      </c>
+      <c r="D8" t="n">
         <v>200</v>
       </c>
     </row>
     <row r="9" spans="1:4">
-      <c r="A9">
-        <v>-90</v>
-      </c>
-      <c r="B9" s="2">
+      <c r="A9" t="n">
+        <v>-90</v>
+      </c>
+      <c r="B9" s="2" t="n">
         <v>40582</v>
       </c>
-      <c r="C9">
-        <v>110</v>
-      </c>
-      <c r="D9">
+      <c r="C9" t="n">
+        <v>110</v>
+      </c>
+      <c r="D9" t="n">
         <v>200</v>
       </c>
     </row>
     <row r="10" spans="1:4">
-      <c r="A10">
-        <v>-90</v>
-      </c>
-      <c r="B10" s="2">
+      <c r="A10" t="n">
+        <v>-90</v>
+      </c>
+      <c r="B10" s="2" t="n">
         <v>40583</v>
       </c>
-      <c r="C10">
-        <v>110</v>
-      </c>
-      <c r="D10">
+      <c r="C10" t="n">
+        <v>110</v>
+      </c>
+      <c r="D10" t="n">
         <v>200</v>
       </c>
     </row>
     <row r="11" spans="1:4">
-      <c r="A11">
-        <v>-90</v>
-      </c>
-      <c r="B11" s="2">
+      <c r="A11" t="n">
+        <v>-90</v>
+      </c>
+      <c r="B11" s="2" t="n">
         <v>40584</v>
       </c>
-      <c r="C11">
-        <v>110</v>
-      </c>
-      <c r="D11">
+      <c r="C11" t="n">
+        <v>110</v>
+      </c>
+      <c r="D11" t="n">
         <v>200</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Changes for fixing tests
</commit_message>
<xml_diff>
--- a/test-data/input/test-data-input-xls-mult-feb.xlsx
+++ b/test-data/input/test-data-input-xls-mult-feb.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
-  <workbookPr defaultThemeVersion="124226"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <workbookPr/>
+  <workbookProtection/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
+  <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="4">
   <si>
     <t>cost</t>
   </si>
@@ -34,28 +35,23 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="YYYY-MM-DD HH:MM:SS"/>
+    <numFmt formatCode="yyyy-mm-dd h:mm:ss" numFmtId="164"/>
   </numFmts>
   <fonts count="2">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
+      <b val="1"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -70,36 +66,27 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="3">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf applyAlignment="1" borderId="1" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="164" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="0" hidden="0" name="Normal" xfId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
 </styleSheet>
 </file>
 
@@ -387,12 +374,18 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
@@ -409,157 +402,163 @@
       </c>
     </row>
     <row r="2" spans="1:4">
-      <c r="A2">
-        <v>-90</v>
-      </c>
-      <c r="B2" s="2">
+      <c r="A2" t="n">
+        <v>-90</v>
+      </c>
+      <c r="B2" s="2" t="n">
         <v>40575</v>
       </c>
-      <c r="C2">
-        <v>110</v>
-      </c>
-      <c r="D2">
+      <c r="C2" t="n">
+        <v>110</v>
+      </c>
+      <c r="D2" t="n">
         <v>200</v>
       </c>
     </row>
     <row r="3" spans="1:4">
-      <c r="A3">
-        <v>-90</v>
-      </c>
-      <c r="B3" s="2">
+      <c r="A3" t="n">
+        <v>-90</v>
+      </c>
+      <c r="B3" s="2" t="n">
         <v>40576</v>
       </c>
-      <c r="C3">
-        <v>110</v>
-      </c>
-      <c r="D3">
+      <c r="C3" t="n">
+        <v>110</v>
+      </c>
+      <c r="D3" t="n">
         <v>200</v>
       </c>
     </row>
     <row r="4" spans="1:4">
-      <c r="A4">
-        <v>-90</v>
-      </c>
-      <c r="B4" s="2">
+      <c r="A4" t="n">
+        <v>-90</v>
+      </c>
+      <c r="B4" s="2" t="n">
         <v>40577</v>
       </c>
-      <c r="C4">
-        <v>110</v>
-      </c>
-      <c r="D4">
+      <c r="C4" t="n">
+        <v>110</v>
+      </c>
+      <c r="D4" t="n">
         <v>200</v>
       </c>
     </row>
     <row r="5" spans="1:4">
-      <c r="A5">
-        <v>-90</v>
-      </c>
-      <c r="B5" s="2">
+      <c r="A5" t="n">
+        <v>-90</v>
+      </c>
+      <c r="B5" s="2" t="n">
         <v>40578</v>
       </c>
-      <c r="C5">
-        <v>110</v>
-      </c>
-      <c r="D5">
+      <c r="C5" t="n">
+        <v>110</v>
+      </c>
+      <c r="D5" t="n">
         <v>200</v>
       </c>
     </row>
     <row r="6" spans="1:4">
-      <c r="A6">
-        <v>-90</v>
-      </c>
-      <c r="B6" s="2">
+      <c r="A6" t="n">
+        <v>-90</v>
+      </c>
+      <c r="B6" s="2" t="n">
         <v>40579</v>
       </c>
-      <c r="C6">
-        <v>110</v>
-      </c>
-      <c r="D6">
+      <c r="C6" t="n">
+        <v>110</v>
+      </c>
+      <c r="D6" t="n">
         <v>200</v>
       </c>
     </row>
     <row r="7" spans="1:4">
-      <c r="A7">
-        <v>-90</v>
-      </c>
-      <c r="B7" s="2">
+      <c r="A7" t="n">
+        <v>-90</v>
+      </c>
+      <c r="B7" s="2" t="n">
         <v>40580</v>
       </c>
-      <c r="C7">
-        <v>110</v>
-      </c>
-      <c r="D7">
+      <c r="C7" t="n">
+        <v>110</v>
+      </c>
+      <c r="D7" t="n">
         <v>200</v>
       </c>
     </row>
     <row r="8" spans="1:4">
-      <c r="A8">
-        <v>-90</v>
-      </c>
-      <c r="B8" s="2">
+      <c r="A8" t="n">
+        <v>-90</v>
+      </c>
+      <c r="B8" s="2" t="n">
         <v>40581</v>
       </c>
-      <c r="C8">
-        <v>110</v>
-      </c>
-      <c r="D8">
+      <c r="C8" t="n">
+        <v>110</v>
+      </c>
+      <c r="D8" t="n">
         <v>200</v>
       </c>
     </row>
     <row r="9" spans="1:4">
-      <c r="A9">
-        <v>-90</v>
-      </c>
-      <c r="B9" s="2">
+      <c r="A9" t="n">
+        <v>-90</v>
+      </c>
+      <c r="B9" s="2" t="n">
         <v>40582</v>
       </c>
-      <c r="C9">
-        <v>110</v>
-      </c>
-      <c r="D9">
+      <c r="C9" t="n">
+        <v>110</v>
+      </c>
+      <c r="D9" t="n">
         <v>200</v>
       </c>
     </row>
     <row r="10" spans="1:4">
-      <c r="A10">
-        <v>-90</v>
-      </c>
-      <c r="B10" s="2">
+      <c r="A10" t="n">
+        <v>-90</v>
+      </c>
+      <c r="B10" s="2" t="n">
         <v>40583</v>
       </c>
-      <c r="C10">
-        <v>110</v>
-      </c>
-      <c r="D10">
+      <c r="C10" t="n">
+        <v>110</v>
+      </c>
+      <c r="D10" t="n">
         <v>200</v>
       </c>
     </row>
     <row r="11" spans="1:4">
-      <c r="A11">
-        <v>-90</v>
-      </c>
-      <c r="B11" s="2">
+      <c r="A11" t="n">
+        <v>-90</v>
+      </c>
+      <c r="B11" s="2" t="n">
         <v>40584</v>
       </c>
-      <c r="C11">
-        <v>110</v>
-      </c>
-      <c r="D11">
+      <c r="C11" t="n">
+        <v>110</v>
+      </c>
+      <c r="D11" t="n">
         <v>200</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
@@ -576,146 +575,146 @@
       </c>
     </row>
     <row r="2" spans="1:4">
-      <c r="A2">
-        <v>-90</v>
-      </c>
-      <c r="B2" s="2">
+      <c r="A2" t="n">
+        <v>-90</v>
+      </c>
+      <c r="B2" s="2" t="n">
         <v>40575</v>
       </c>
-      <c r="C2">
-        <v>110</v>
-      </c>
-      <c r="D2">
+      <c r="C2" t="n">
+        <v>110</v>
+      </c>
+      <c r="D2" t="n">
         <v>200</v>
       </c>
     </row>
     <row r="3" spans="1:4">
-      <c r="A3">
-        <v>-90</v>
-      </c>
-      <c r="B3" s="2">
+      <c r="A3" t="n">
+        <v>-90</v>
+      </c>
+      <c r="B3" s="2" t="n">
         <v>40576</v>
       </c>
-      <c r="C3">
-        <v>110</v>
-      </c>
-      <c r="D3">
+      <c r="C3" t="n">
+        <v>110</v>
+      </c>
+      <c r="D3" t="n">
         <v>200</v>
       </c>
     </row>
     <row r="4" spans="1:4">
-      <c r="A4">
-        <v>-90</v>
-      </c>
-      <c r="B4" s="2">
+      <c r="A4" t="n">
+        <v>-90</v>
+      </c>
+      <c r="B4" s="2" t="n">
         <v>40577</v>
       </c>
-      <c r="C4">
-        <v>110</v>
-      </c>
-      <c r="D4">
+      <c r="C4" t="n">
+        <v>110</v>
+      </c>
+      <c r="D4" t="n">
         <v>200</v>
       </c>
     </row>
     <row r="5" spans="1:4">
-      <c r="A5">
-        <v>-90</v>
-      </c>
-      <c r="B5" s="2">
+      <c r="A5" t="n">
+        <v>-90</v>
+      </c>
+      <c r="B5" s="2" t="n">
         <v>40578</v>
       </c>
-      <c r="C5">
-        <v>110</v>
-      </c>
-      <c r="D5">
+      <c r="C5" t="n">
+        <v>110</v>
+      </c>
+      <c r="D5" t="n">
         <v>200</v>
       </c>
     </row>
     <row r="6" spans="1:4">
-      <c r="A6">
-        <v>-90</v>
-      </c>
-      <c r="B6" s="2">
+      <c r="A6" t="n">
+        <v>-90</v>
+      </c>
+      <c r="B6" s="2" t="n">
         <v>40579</v>
       </c>
-      <c r="C6">
-        <v>110</v>
-      </c>
-      <c r="D6">
+      <c r="C6" t="n">
+        <v>110</v>
+      </c>
+      <c r="D6" t="n">
         <v>200</v>
       </c>
     </row>
     <row r="7" spans="1:4">
-      <c r="A7">
-        <v>-90</v>
-      </c>
-      <c r="B7" s="2">
+      <c r="A7" t="n">
+        <v>-90</v>
+      </c>
+      <c r="B7" s="2" t="n">
         <v>40580</v>
       </c>
-      <c r="C7">
-        <v>110</v>
-      </c>
-      <c r="D7">
+      <c r="C7" t="n">
+        <v>110</v>
+      </c>
+      <c r="D7" t="n">
         <v>200</v>
       </c>
     </row>
     <row r="8" spans="1:4">
-      <c r="A8">
-        <v>-90</v>
-      </c>
-      <c r="B8" s="2">
+      <c r="A8" t="n">
+        <v>-90</v>
+      </c>
+      <c r="B8" s="2" t="n">
         <v>40581</v>
       </c>
-      <c r="C8">
-        <v>110</v>
-      </c>
-      <c r="D8">
+      <c r="C8" t="n">
+        <v>110</v>
+      </c>
+      <c r="D8" t="n">
         <v>200</v>
       </c>
     </row>
     <row r="9" spans="1:4">
-      <c r="A9">
-        <v>-90</v>
-      </c>
-      <c r="B9" s="2">
+      <c r="A9" t="n">
+        <v>-90</v>
+      </c>
+      <c r="B9" s="2" t="n">
         <v>40582</v>
       </c>
-      <c r="C9">
-        <v>110</v>
-      </c>
-      <c r="D9">
+      <c r="C9" t="n">
+        <v>110</v>
+      </c>
+      <c r="D9" t="n">
         <v>200</v>
       </c>
     </row>
     <row r="10" spans="1:4">
-      <c r="A10">
-        <v>-90</v>
-      </c>
-      <c r="B10" s="2">
+      <c r="A10" t="n">
+        <v>-90</v>
+      </c>
+      <c r="B10" s="2" t="n">
         <v>40583</v>
       </c>
-      <c r="C10">
-        <v>110</v>
-      </c>
-      <c r="D10">
+      <c r="C10" t="n">
+        <v>110</v>
+      </c>
+      <c r="D10" t="n">
         <v>200</v>
       </c>
     </row>
     <row r="11" spans="1:4">
-      <c r="A11">
-        <v>-90</v>
-      </c>
-      <c r="B11" s="2">
+      <c r="A11" t="n">
+        <v>-90</v>
+      </c>
+      <c r="B11" s="2" t="n">
         <v>40584</v>
       </c>
-      <c r="C11">
-        <v>110</v>
-      </c>
-      <c r="D11">
+      <c r="C11" t="n">
+        <v>110</v>
+      </c>
+      <c r="D11" t="n">
         <v>200</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Changes for Trello tasks regarding overwrite and if_exists
</commit_message>
<xml_diff>
--- a/test-data/input/test-data-input-xls-mult-feb.xlsx
+++ b/test-data/input/test-data-input-xls-mult-feb.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
-  <workbookPr defaultThemeVersion="124226"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <workbookPr/>
+  <workbookProtection/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
+  <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="4">
   <si>
     <t>cost</t>
   </si>
@@ -34,28 +35,23 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="YYYY-MM-DD HH:MM:SS"/>
+    <numFmt formatCode="yyyy-mm-dd h:mm:ss" numFmtId="164"/>
   </numFmts>
   <fonts count="2">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
+      <b val="1"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -70,36 +66,27 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="3">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf applyAlignment="1" borderId="1" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="164" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="0" hidden="0" name="Normal" xfId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
 </styleSheet>
 </file>
 
@@ -387,12 +374,18 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
@@ -409,157 +402,163 @@
       </c>
     </row>
     <row r="2" spans="1:4">
-      <c r="A2">
-        <v>-90</v>
-      </c>
-      <c r="B2" s="2">
+      <c r="A2" t="n">
+        <v>-90</v>
+      </c>
+      <c r="B2" s="2" t="n">
         <v>40575</v>
       </c>
-      <c r="C2">
-        <v>110</v>
-      </c>
-      <c r="D2">
+      <c r="C2" t="n">
+        <v>110</v>
+      </c>
+      <c r="D2" t="n">
         <v>200</v>
       </c>
     </row>
     <row r="3" spans="1:4">
-      <c r="A3">
-        <v>-90</v>
-      </c>
-      <c r="B3" s="2">
+      <c r="A3" t="n">
+        <v>-90</v>
+      </c>
+      <c r="B3" s="2" t="n">
         <v>40576</v>
       </c>
-      <c r="C3">
-        <v>110</v>
-      </c>
-      <c r="D3">
+      <c r="C3" t="n">
+        <v>110</v>
+      </c>
+      <c r="D3" t="n">
         <v>200</v>
       </c>
     </row>
     <row r="4" spans="1:4">
-      <c r="A4">
-        <v>-90</v>
-      </c>
-      <c r="B4" s="2">
+      <c r="A4" t="n">
+        <v>-90</v>
+      </c>
+      <c r="B4" s="2" t="n">
         <v>40577</v>
       </c>
-      <c r="C4">
-        <v>110</v>
-      </c>
-      <c r="D4">
+      <c r="C4" t="n">
+        <v>110</v>
+      </c>
+      <c r="D4" t="n">
         <v>200</v>
       </c>
     </row>
     <row r="5" spans="1:4">
-      <c r="A5">
-        <v>-90</v>
-      </c>
-      <c r="B5" s="2">
+      <c r="A5" t="n">
+        <v>-90</v>
+      </c>
+      <c r="B5" s="2" t="n">
         <v>40578</v>
       </c>
-      <c r="C5">
-        <v>110</v>
-      </c>
-      <c r="D5">
+      <c r="C5" t="n">
+        <v>110</v>
+      </c>
+      <c r="D5" t="n">
         <v>200</v>
       </c>
     </row>
     <row r="6" spans="1:4">
-      <c r="A6">
-        <v>-90</v>
-      </c>
-      <c r="B6" s="2">
+      <c r="A6" t="n">
+        <v>-90</v>
+      </c>
+      <c r="B6" s="2" t="n">
         <v>40579</v>
       </c>
-      <c r="C6">
-        <v>110</v>
-      </c>
-      <c r="D6">
+      <c r="C6" t="n">
+        <v>110</v>
+      </c>
+      <c r="D6" t="n">
         <v>200</v>
       </c>
     </row>
     <row r="7" spans="1:4">
-      <c r="A7">
-        <v>-90</v>
-      </c>
-      <c r="B7" s="2">
+      <c r="A7" t="n">
+        <v>-90</v>
+      </c>
+      <c r="B7" s="2" t="n">
         <v>40580</v>
       </c>
-      <c r="C7">
-        <v>110</v>
-      </c>
-      <c r="D7">
+      <c r="C7" t="n">
+        <v>110</v>
+      </c>
+      <c r="D7" t="n">
         <v>200</v>
       </c>
     </row>
     <row r="8" spans="1:4">
-      <c r="A8">
-        <v>-90</v>
-      </c>
-      <c r="B8" s="2">
+      <c r="A8" t="n">
+        <v>-90</v>
+      </c>
+      <c r="B8" s="2" t="n">
         <v>40581</v>
       </c>
-      <c r="C8">
-        <v>110</v>
-      </c>
-      <c r="D8">
+      <c r="C8" t="n">
+        <v>110</v>
+      </c>
+      <c r="D8" t="n">
         <v>200</v>
       </c>
     </row>
     <row r="9" spans="1:4">
-      <c r="A9">
-        <v>-90</v>
-      </c>
-      <c r="B9" s="2">
+      <c r="A9" t="n">
+        <v>-90</v>
+      </c>
+      <c r="B9" s="2" t="n">
         <v>40582</v>
       </c>
-      <c r="C9">
-        <v>110</v>
-      </c>
-      <c r="D9">
+      <c r="C9" t="n">
+        <v>110</v>
+      </c>
+      <c r="D9" t="n">
         <v>200</v>
       </c>
     </row>
     <row r="10" spans="1:4">
-      <c r="A10">
-        <v>-90</v>
-      </c>
-      <c r="B10" s="2">
+      <c r="A10" t="n">
+        <v>-90</v>
+      </c>
+      <c r="B10" s="2" t="n">
         <v>40583</v>
       </c>
-      <c r="C10">
-        <v>110</v>
-      </c>
-      <c r="D10">
+      <c r="C10" t="n">
+        <v>110</v>
+      </c>
+      <c r="D10" t="n">
         <v>200</v>
       </c>
     </row>
     <row r="11" spans="1:4">
-      <c r="A11">
-        <v>-90</v>
-      </c>
-      <c r="B11" s="2">
+      <c r="A11" t="n">
+        <v>-90</v>
+      </c>
+      <c r="B11" s="2" t="n">
         <v>40584</v>
       </c>
-      <c r="C11">
-        <v>110</v>
-      </c>
-      <c r="D11">
+      <c r="C11" t="n">
+        <v>110</v>
+      </c>
+      <c r="D11" t="n">
         <v>200</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
@@ -576,146 +575,146 @@
       </c>
     </row>
     <row r="2" spans="1:4">
-      <c r="A2">
-        <v>-90</v>
-      </c>
-      <c r="B2" s="2">
+      <c r="A2" t="n">
+        <v>-90</v>
+      </c>
+      <c r="B2" s="2" t="n">
         <v>40575</v>
       </c>
-      <c r="C2">
-        <v>110</v>
-      </c>
-      <c r="D2">
+      <c r="C2" t="n">
+        <v>110</v>
+      </c>
+      <c r="D2" t="n">
         <v>200</v>
       </c>
     </row>
     <row r="3" spans="1:4">
-      <c r="A3">
-        <v>-90</v>
-      </c>
-      <c r="B3" s="2">
+      <c r="A3" t="n">
+        <v>-90</v>
+      </c>
+      <c r="B3" s="2" t="n">
         <v>40576</v>
       </c>
-      <c r="C3">
-        <v>110</v>
-      </c>
-      <c r="D3">
+      <c r="C3" t="n">
+        <v>110</v>
+      </c>
+      <c r="D3" t="n">
         <v>200</v>
       </c>
     </row>
     <row r="4" spans="1:4">
-      <c r="A4">
-        <v>-90</v>
-      </c>
-      <c r="B4" s="2">
+      <c r="A4" t="n">
+        <v>-90</v>
+      </c>
+      <c r="B4" s="2" t="n">
         <v>40577</v>
       </c>
-      <c r="C4">
-        <v>110</v>
-      </c>
-      <c r="D4">
+      <c r="C4" t="n">
+        <v>110</v>
+      </c>
+      <c r="D4" t="n">
         <v>200</v>
       </c>
     </row>
     <row r="5" spans="1:4">
-      <c r="A5">
-        <v>-90</v>
-      </c>
-      <c r="B5" s="2">
+      <c r="A5" t="n">
+        <v>-90</v>
+      </c>
+      <c r="B5" s="2" t="n">
         <v>40578</v>
       </c>
-      <c r="C5">
-        <v>110</v>
-      </c>
-      <c r="D5">
+      <c r="C5" t="n">
+        <v>110</v>
+      </c>
+      <c r="D5" t="n">
         <v>200</v>
       </c>
     </row>
     <row r="6" spans="1:4">
-      <c r="A6">
-        <v>-90</v>
-      </c>
-      <c r="B6" s="2">
+      <c r="A6" t="n">
+        <v>-90</v>
+      </c>
+      <c r="B6" s="2" t="n">
         <v>40579</v>
       </c>
-      <c r="C6">
-        <v>110</v>
-      </c>
-      <c r="D6">
+      <c r="C6" t="n">
+        <v>110</v>
+      </c>
+      <c r="D6" t="n">
         <v>200</v>
       </c>
     </row>
     <row r="7" spans="1:4">
-      <c r="A7">
-        <v>-90</v>
-      </c>
-      <c r="B7" s="2">
+      <c r="A7" t="n">
+        <v>-90</v>
+      </c>
+      <c r="B7" s="2" t="n">
         <v>40580</v>
       </c>
-      <c r="C7">
-        <v>110</v>
-      </c>
-      <c r="D7">
+      <c r="C7" t="n">
+        <v>110</v>
+      </c>
+      <c r="D7" t="n">
         <v>200</v>
       </c>
     </row>
     <row r="8" spans="1:4">
-      <c r="A8">
-        <v>-90</v>
-      </c>
-      <c r="B8" s="2">
+      <c r="A8" t="n">
+        <v>-90</v>
+      </c>
+      <c r="B8" s="2" t="n">
         <v>40581</v>
       </c>
-      <c r="C8">
-        <v>110</v>
-      </c>
-      <c r="D8">
+      <c r="C8" t="n">
+        <v>110</v>
+      </c>
+      <c r="D8" t="n">
         <v>200</v>
       </c>
     </row>
     <row r="9" spans="1:4">
-      <c r="A9">
-        <v>-90</v>
-      </c>
-      <c r="B9" s="2">
+      <c r="A9" t="n">
+        <v>-90</v>
+      </c>
+      <c r="B9" s="2" t="n">
         <v>40582</v>
       </c>
-      <c r="C9">
-        <v>110</v>
-      </c>
-      <c r="D9">
+      <c r="C9" t="n">
+        <v>110</v>
+      </c>
+      <c r="D9" t="n">
         <v>200</v>
       </c>
     </row>
     <row r="10" spans="1:4">
-      <c r="A10">
-        <v>-90</v>
-      </c>
-      <c r="B10" s="2">
+      <c r="A10" t="n">
+        <v>-90</v>
+      </c>
+      <c r="B10" s="2" t="n">
         <v>40583</v>
       </c>
-      <c r="C10">
-        <v>110</v>
-      </c>
-      <c r="D10">
+      <c r="C10" t="n">
+        <v>110</v>
+      </c>
+      <c r="D10" t="n">
         <v>200</v>
       </c>
     </row>
     <row r="11" spans="1:4">
-      <c r="A11">
-        <v>-90</v>
-      </c>
-      <c r="B11" s="2">
+      <c r="A11" t="n">
+        <v>-90</v>
+      </c>
+      <c r="B11" s="2" t="n">
         <v>40584</v>
       </c>
-      <c r="C11">
-        <v>110</v>
-      </c>
-      <c r="D11">
+      <c r="C11" t="n">
+        <v>110</v>
+      </c>
+      <c r="D11" t="n">
         <v>200</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>
 </file>
</xml_diff>